<commit_message>
Updated quick quote for both qa and stg
</commit_message>
<xml_diff>
--- a/testdata/FCfiles/stg/ManageProducts/ManageProducts.xlsx
+++ b/testdata/FCfiles/stg/ManageProducts/ManageProducts.xlsx
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="320" uniqueCount="294">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="326" uniqueCount="300">
   <si>
     <t>Other</t>
   </si>
@@ -907,6 +907,24 @@
   </si>
   <si>
     <t>prodAMDv</t>
+  </si>
+  <si>
+    <t>prodVVhf</t>
+  </si>
+  <si>
+    <t>prodFsyH</t>
+  </si>
+  <si>
+    <t>prodPcCp</t>
+  </si>
+  <si>
+    <t>prodpLJJ</t>
+  </si>
+  <si>
+    <t>prodDBms</t>
+  </si>
+  <si>
+    <t>prodXvSh</t>
   </si>
 </sst>
 </file>
@@ -937,7 +955,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="508">
+  <fills count="520">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -3474,8 +3492,68 @@
         <fgColor indexed="9"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="none">
+        <fgColor indexed="9"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor indexed="9"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="none">
+        <fgColor indexed="9"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor indexed="9"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="none">
+        <fgColor indexed="9"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor indexed="9"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="none">
+        <fgColor indexed="9"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor indexed="9"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="none">
+        <fgColor indexed="9"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor indexed="9"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="none">
+        <fgColor indexed="9"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor indexed="9"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="512">
+  <borders count="524">
     <border>
       <left/>
       <right/>
@@ -5420,11 +5498,53 @@
       <top style="thin"/>
       <bottom style="thin"/>
     </border>
+    <border>
+      <top style="thin"/>
+    </border>
+    <border>
+      <top style="thin"/>
+      <bottom style="thin"/>
+    </border>
+    <border>
+      <top style="thin"/>
+    </border>
+    <border>
+      <top style="thin"/>
+      <bottom style="thin"/>
+    </border>
+    <border>
+      <top style="thin"/>
+    </border>
+    <border>
+      <top style="thin"/>
+      <bottom style="thin"/>
+    </border>
+    <border>
+      <top style="thin"/>
+    </border>
+    <border>
+      <top style="thin"/>
+      <bottom style="thin"/>
+    </border>
+    <border>
+      <top style="thin"/>
+    </border>
+    <border>
+      <top style="thin"/>
+      <bottom style="thin"/>
+    </border>
+    <border>
+      <top style="thin"/>
+    </border>
+    <border>
+      <top style="thin"/>
+      <bottom style="thin"/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf borderId="0" fillId="0" fontId="0" numFmtId="0"/>
   </cellStyleXfs>
-  <cellXfs count="273">
+  <cellXfs count="279">
     <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0"/>
     <xf applyBorder="1" borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0"/>
     <xf applyAlignment="1" applyBorder="1" applyFont="1" borderId="2" fillId="0" fontId="2" numFmtId="0" xfId="0">
@@ -5725,7 +5845,13 @@
     <xf applyBorder="true" applyFill="true" borderId="505" fillId="501" fontId="0" numFmtId="0" xfId="0"/>
     <xf applyBorder="true" applyFill="true" borderId="507" fillId="503" fontId="0" numFmtId="0" xfId="0"/>
     <xf applyBorder="true" applyFill="true" borderId="509" fillId="505" fontId="0" numFmtId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="0" fillId="507" borderId="511" xfId="0" applyFill="true" applyBorder="true"/>
+    <xf applyBorder="true" applyFill="true" borderId="511" fillId="507" fontId="0" numFmtId="0" xfId="0"/>
+    <xf applyBorder="true" applyFill="true" borderId="513" fillId="509" fontId="0" numFmtId="0" xfId="0"/>
+    <xf applyBorder="true" applyFill="true" borderId="515" fillId="511" fontId="0" numFmtId="0" xfId="0"/>
+    <xf applyBorder="true" applyFill="true" borderId="517" fillId="513" fontId="0" numFmtId="0" xfId="0"/>
+    <xf applyBorder="true" applyFill="true" borderId="519" fillId="515" fontId="0" numFmtId="0" xfId="0"/>
+    <xf applyBorder="true" applyFill="true" borderId="521" fillId="517" fontId="0" numFmtId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="519" borderId="523" xfId="0" applyFill="true" applyBorder="true"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle builtinId="0" name="Normal" xfId="0"/>
@@ -6095,8 +6221,8 @@
       <c r="A2" s="6" t="s">
         <v>29</v>
       </c>
-      <c r="B2" s="272" t="s">
-        <v>293</v>
+      <c r="B2" s="278" t="s">
+        <v>299</v>
       </c>
       <c r="C2" s="7" t="s">
         <v>17</v>
@@ -6133,8 +6259,8 @@
       <c r="A3" s="6" t="s">
         <v>30</v>
       </c>
-      <c r="B3" s="269" t="s">
-        <v>290</v>
+      <c r="B3" s="275" t="s">
+        <v>296</v>
       </c>
       <c r="C3" s="7" t="s">
         <v>17</v>
@@ -6227,8 +6353,8 @@
       <c r="A5" s="6" t="s">
         <v>32</v>
       </c>
-      <c r="B5" s="270" t="s">
-        <v>291</v>
+      <c r="B5" s="276" t="s">
+        <v>297</v>
       </c>
       <c r="C5" s="7" t="s">
         <v>17</v>

</xml_diff>